<commit_message>
Minor formatting and content fixes
</commit_message>
<xml_diff>
--- a/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/01-Basic-Units-of-Information-Measurement/Resources/edinici.xlsx
+++ b/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/01-Basic-Units-of-Information-Measurement/Resources/edinici.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vs project\GitHub\School-Programming\Courses\Computer-Modeling-and-IT\Computer-Modeling-and-IT-6-Class\01-Basic-Units-of-Information-Measurement\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrinamehandzhiyska/Documents/GitHub/School-Programming/Courses/Computer-Modeling-and-IT/Computer-Modeling-and-IT-6-Class/01-Basic-Units-of-Information-Measurement/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80DB06-B652-5044-84D8-36AFBF352631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,21 +396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -420,7 +421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -431,39 +432,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>